<commit_message>
Add locations for Ribleaf and Fool's Parsley
</commit_message>
<xml_diff>
--- a/W3EEIngredients.xlsx
+++ b/W3EEIngredients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A095969B-F679-4534-B969-BBA44A1F50A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC713DD2-46EE-47EE-A371-1D6B166E659E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7695" windowWidth="16440" windowHeight="28590" xr2:uid="{471E009D-222C-402C-AA03-67F028A6D488}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>Monster Wing Sample</t>
+  </si>
+  <si>
+    <t>Drahim Castle (west fields)</t>
+  </si>
+  <si>
+    <t>Mulbrydale (surrounding roads), Woesong Bridge (west fields)</t>
   </si>
 </sst>
 </file>
@@ -871,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C10D996-40BF-4304-BA54-82664D0442EC}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2488,6 +2494,9 @@
       </c>
       <c r="D96" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>